<commit_message>
finished occupation classification (each state)
</commit_message>
<xml_diff>
--- a/S2022/comparison_between_debt_holders/avg_debt_occupation/FinishedSpreadsheets/OccupationsCT.xlsx
+++ b/S2022/comparison_between_debt_holders/avg_debt_occupation/FinishedSpreadsheets/OccupationsCT.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>occupation</t>
   </si>
@@ -85,6 +85,9 @@
     <t>leather dresser</t>
   </si>
   <si>
+    <t>mariner</t>
+  </si>
+  <si>
     <t>merchant</t>
   </si>
   <si>
@@ -100,10 +103,16 @@
     <t>post rider</t>
   </si>
   <si>
+    <t>printer</t>
+  </si>
+  <si>
     <t>proprietors</t>
   </si>
   <si>
     <t>sadler</t>
+  </si>
+  <si>
+    <t>school committee</t>
   </si>
   <si>
     <t>school master</t>
@@ -500,7 +509,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -610,7 +619,7 @@
         <v>10</v>
       </c>
       <c r="C10">
-        <v>1935.06</v>
+        <v>863.41</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -753,7 +762,7 @@
         <v>23</v>
       </c>
       <c r="C23">
-        <v>63765.00000000001</v>
+        <v>3831.05</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -764,7 +773,7 @@
         <v>24</v>
       </c>
       <c r="C24">
-        <v>18.99</v>
+        <v>63765.00000000001</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -775,7 +784,7 @@
         <v>25</v>
       </c>
       <c r="C25">
-        <v>211.38</v>
+        <v>18.99</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -786,7 +795,7 @@
         <v>26</v>
       </c>
       <c r="C26">
-        <v>1303.46</v>
+        <v>211.38</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -797,7 +806,7 @@
         <v>27</v>
       </c>
       <c r="C27">
-        <v>676.91</v>
+        <v>1303.46</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -808,7 +817,7 @@
         <v>28</v>
       </c>
       <c r="C28">
-        <v>276.9</v>
+        <v>676.91</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -819,7 +828,7 @@
         <v>29</v>
       </c>
       <c r="C29">
-        <v>3524.74</v>
+        <v>204.78</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -830,7 +839,7 @@
         <v>30</v>
       </c>
       <c r="C30">
-        <v>2213.75</v>
+        <v>276.9</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -841,7 +850,7 @@
         <v>31</v>
       </c>
       <c r="C31">
-        <v>512.45</v>
+        <v>3524.74</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -852,7 +861,7 @@
         <v>32</v>
       </c>
       <c r="C32">
-        <v>533.33</v>
+        <v>1071.65</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -863,7 +872,7 @@
         <v>33</v>
       </c>
       <c r="C33">
-        <v>1345.46</v>
+        <v>2213.75</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -874,7 +883,7 @@
         <v>34</v>
       </c>
       <c r="C34">
-        <v>78.48</v>
+        <v>512.45</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -885,7 +894,7 @@
         <v>35</v>
       </c>
       <c r="C35">
-        <v>5767.41</v>
+        <v>533.33</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -896,7 +905,7 @@
         <v>36</v>
       </c>
       <c r="C36">
-        <v>713.0599999999999</v>
+        <v>1345.46</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -907,7 +916,7 @@
         <v>37</v>
       </c>
       <c r="C37">
-        <v>209.81</v>
+        <v>78.48</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -918,7 +927,7 @@
         <v>38</v>
       </c>
       <c r="C38">
-        <v>9454.129999999999</v>
+        <v>1731.58</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -929,7 +938,7 @@
         <v>39</v>
       </c>
       <c r="C39">
-        <v>15387.15</v>
+        <v>713.0599999999999</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -940,7 +949,7 @@
         <v>40</v>
       </c>
       <c r="C40">
-        <v>6488.11</v>
+        <v>209.81</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -951,7 +960,7 @@
         <v>41</v>
       </c>
       <c r="C41">
-        <v>63.64</v>
+        <v>9454.129999999999</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -962,6 +971,39 @@
         <v>42</v>
       </c>
       <c r="C42">
+        <v>15387.15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="1">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>43</v>
+      </c>
+      <c r="C43">
+        <v>6488.11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="1">
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
+        <v>44</v>
+      </c>
+      <c r="C44">
+        <v>63.64</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="1">
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>45</v>
+      </c>
+      <c r="C45">
         <v>64.54000000000001</v>
       </c>
     </row>

</xml_diff>